<commit_message>
add compv2 excell 清算数据
</commit_message>
<xml_diff>
--- a/someContract/errorContract/存款借贷类/lendfME/compV1清算模型数据.xlsx
+++ b/someContract/errorContract/存款借贷类/lendfME/compV1清算模型数据.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\projectTest\solidityTest\someContract\errorContract\存款借贷类\lendfME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58EAE5E9-7F6D-4225-B573-1A31602BB5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C940CD3A-631D-40D2-856E-01F8E3AE97D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84F9BC4C-BCA9-402D-9630-9AEF0368CF2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{84F9BC4C-BCA9-402D-9630-9AEF0368CF2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2_x0009__x0009_v2_x0009__x0009__x0009__x0009__x0009__x0009__x0009__x0009__x0009__x0009__x0009__x0009_" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>这两个值哪个小 取哪个 再和优惠还款至等额 比较</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -126,6 +127,42 @@
     <t>然后除以1.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>v2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>liquidationIncentiveMantissa 清算系数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>借贷的一半</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取抵押品数量</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>剩借贷</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>剩抵押</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>清算后短缺</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>清算前短缺</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>多次清算 使用短缺至0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -207,12 +244,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -221,6 +252,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C517679-058B-4FBC-9EE7-37957E23084B}">
   <dimension ref="B1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -568,14 +605,14 @@
       <c r="C1" s="2"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="L7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="5"/>
+      <c r="L7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="L8" s="2" t="s">
@@ -618,12 +655,12 @@
       </c>
     </row>
     <row r="11" spans="2:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="N11" s="6" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="N11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O11" s="2" t="s">
@@ -865,7 +902,7 @@
         <f t="shared" si="3"/>
         <v>80.808080808080803</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="5">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
@@ -1255,12 +1292,12 @@
       </c>
     </row>
     <row r="30" spans="7:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="N30" s="6" t="s">
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="N30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O30" s="2" t="s">
@@ -1499,7 +1536,7 @@
         <f t="shared" si="14"/>
         <v>145.45454545454544</v>
       </c>
-      <c r="Q35" s="7">
+      <c r="Q35" s="5">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -2128,4 +2165,1368 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AA9B81-A43C-43E1-AC49-7361BDE9FDBA}">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>340</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E6" si="0">D5/F5</f>
+        <v>4.25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>1.08</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>D5/2</f>
+        <v>170</v>
+      </c>
+      <c r="K5">
+        <f>J5/1*H5</f>
+        <v>183.60000000000002</v>
+      </c>
+      <c r="L5">
+        <f>D5-J5</f>
+        <v>170</v>
+      </c>
+      <c r="M5">
+        <f>C5-K5</f>
+        <v>816.4</v>
+      </c>
+      <c r="N5">
+        <f>IF(M5*1/I5-J5&gt;0,0,-M5*1/I5+J5)</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>IF(C5*1/I5-D5&gt;0,0,-C5*1/I5+D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>400</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>80</v>
+      </c>
+      <c r="H6">
+        <v>1.08</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J17" si="1">D6/2</f>
+        <v>200</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K17" si="2">J6/1*H6</f>
+        <v>216</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L17" si="3">D6-J6</f>
+        <v>200</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M17" si="4">C6-K6</f>
+        <v>784</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N17" si="5">IF(M6*1/I6-J6&gt;0,0,-M6*1/I6+J6)</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O17" si="6">IF(C6*1/I6-D6&gt;0,0,-C6*1/I6+D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>1000</v>
+      </c>
+      <c r="D7">
+        <v>450</v>
+      </c>
+      <c r="E7">
+        <f>D7/F7</f>
+        <v>5.625</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="H7">
+        <v>1.08</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>243.00000000000003</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>757</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8">
+        <f>D8/F8</f>
+        <v>6.25</v>
+      </c>
+      <c r="F8">
+        <v>80</v>
+      </c>
+      <c r="H8">
+        <v>1.08</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>730</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>510</v>
+      </c>
+      <c r="E9">
+        <f>D9/F9</f>
+        <v>6.375</v>
+      </c>
+      <c r="F9">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>1.08</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>275.40000000000003</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>255</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>724.59999999999991</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>540</v>
+      </c>
+      <c r="E10">
+        <f>D10/F10</f>
+        <v>6.75</v>
+      </c>
+      <c r="F10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>1.08</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>291.60000000000002</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>270</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>708.4</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11">
+        <v>550</v>
+      </c>
+      <c r="E11">
+        <f>D11/F11</f>
+        <v>6.875</v>
+      </c>
+      <c r="F11">
+        <v>80</v>
+      </c>
+      <c r="H11">
+        <v>1.08</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>297</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>275</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>703</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>600</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E17" si="7">D12/F12</f>
+        <v>7.5</v>
+      </c>
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="H12">
+        <v>1.08</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>324</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>676</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <v>700</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="7"/>
+        <v>8.75</v>
+      </c>
+      <c r="F13">
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>1.08</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>378</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>622</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>1000</v>
+      </c>
+      <c r="D14">
+        <v>800</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <v>1.08</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>432</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>568</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1000</v>
+      </c>
+      <c r="D15">
+        <v>900</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>11.25</v>
+      </c>
+      <c r="F15">
+        <v>80</v>
+      </c>
+      <c r="H15">
+        <v>1.08</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>486.00000000000006</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>514</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>193</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>1000</v>
+      </c>
+      <c r="D16">
+        <v>1000</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>12.5</v>
+      </c>
+      <c r="F16">
+        <v>80</v>
+      </c>
+      <c r="H16">
+        <v>1.08</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>540</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>460</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>1000</v>
+      </c>
+      <c r="D17">
+        <v>1200</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>80</v>
+      </c>
+      <c r="H17">
+        <v>1.08</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>648</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>352</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>424</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C22" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D22" s="2">
+        <v>340</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E23" si="8">D22/F22</f>
+        <v>4.25</v>
+      </c>
+      <c r="F22" s="2">
+        <v>80</v>
+      </c>
+      <c r="H22">
+        <v>1.08</v>
+      </c>
+      <c r="I22">
+        <v>1.25</v>
+      </c>
+      <c r="J22">
+        <f>D22/2</f>
+        <v>170</v>
+      </c>
+      <c r="K22">
+        <f>J22/1*H22</f>
+        <v>183.60000000000002</v>
+      </c>
+      <c r="L22">
+        <f>D22-J22</f>
+        <v>170</v>
+      </c>
+      <c r="M22">
+        <f>C22-K22</f>
+        <v>816.4</v>
+      </c>
+      <c r="N22">
+        <f>IF(M22*1/I22-L22&gt;0,0,-M22*1/I22+L22)</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>IF(C22*1/I22-D22&gt;0,0,-C22*1/I22+D22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C23" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="2">
+        <v>400</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>80</v>
+      </c>
+      <c r="H23">
+        <v>1.08</v>
+      </c>
+      <c r="I23">
+        <v>1.25</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:J36" si="9">D23/2</f>
+        <v>200</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="K23:K36" si="10">J23/1*H23</f>
+        <v>216</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:L36" si="11">D23-J23</f>
+        <v>200</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:M34" si="12">C23-K23</f>
+        <v>784</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:N36" si="13">IF(M23*1/I23-L23&gt;0,0,-M23*1/I23+L23)</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23:O36" si="14">IF(C23*1/I23-D23&gt;0,0,-C23*1/I23+D23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>1000</v>
+      </c>
+      <c r="D24">
+        <v>450</v>
+      </c>
+      <c r="E24">
+        <f>D24/F24</f>
+        <v>5.625</v>
+      </c>
+      <c r="F24">
+        <v>80</v>
+      </c>
+      <c r="H24">
+        <v>1.08</v>
+      </c>
+      <c r="I24">
+        <v>1.25</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>225</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="10"/>
+        <v>243.00000000000003</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="11"/>
+        <v>225</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="12"/>
+        <v>757</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>1000</v>
+      </c>
+      <c r="D25">
+        <v>500</v>
+      </c>
+      <c r="E25">
+        <f>D25/F25</f>
+        <v>6.25</v>
+      </c>
+      <c r="F25">
+        <v>80</v>
+      </c>
+      <c r="H25">
+        <v>1.08</v>
+      </c>
+      <c r="I25">
+        <v>1.25</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="9"/>
+        <v>250</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="10"/>
+        <v>270</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="11"/>
+        <v>250</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="12"/>
+        <v>730</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>1000</v>
+      </c>
+      <c r="D26">
+        <v>510</v>
+      </c>
+      <c r="E26">
+        <f>D26/F26</f>
+        <v>6.375</v>
+      </c>
+      <c r="F26">
+        <v>80</v>
+      </c>
+      <c r="H26">
+        <v>1.08</v>
+      </c>
+      <c r="I26">
+        <v>1.25</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="9"/>
+        <v>255</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="10"/>
+        <v>275.40000000000003</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="11"/>
+        <v>255</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="12"/>
+        <v>724.59999999999991</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>1000</v>
+      </c>
+      <c r="D27">
+        <v>540</v>
+      </c>
+      <c r="E27">
+        <f>D27/F27</f>
+        <v>6.75</v>
+      </c>
+      <c r="F27">
+        <v>80</v>
+      </c>
+      <c r="H27">
+        <v>1.08</v>
+      </c>
+      <c r="I27">
+        <v>1.25</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="9"/>
+        <v>270</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="10"/>
+        <v>291.60000000000002</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="11"/>
+        <v>270</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="12"/>
+        <v>708.4</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>1000</v>
+      </c>
+      <c r="D28">
+        <v>550</v>
+      </c>
+      <c r="E28">
+        <f>D28/F28</f>
+        <v>6.875</v>
+      </c>
+      <c r="F28">
+        <v>80</v>
+      </c>
+      <c r="H28">
+        <v>1.08</v>
+      </c>
+      <c r="I28">
+        <v>1.25</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="9"/>
+        <v>275</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="10"/>
+        <v>297</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="11"/>
+        <v>275</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="12"/>
+        <v>703</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>1000</v>
+      </c>
+      <c r="D29">
+        <v>600</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E34" si="15">D29/F29</f>
+        <v>7.5</v>
+      </c>
+      <c r="F29">
+        <v>80</v>
+      </c>
+      <c r="H29">
+        <v>1.08</v>
+      </c>
+      <c r="I29">
+        <v>1.25</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="10"/>
+        <v>324</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="11"/>
+        <v>300</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="12"/>
+        <v>676</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1000</v>
+      </c>
+      <c r="D30">
+        <v>700</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="15"/>
+        <v>8.75</v>
+      </c>
+      <c r="F30">
+        <v>80</v>
+      </c>
+      <c r="H30">
+        <v>1.08</v>
+      </c>
+      <c r="I30">
+        <v>1.25</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="9"/>
+        <v>350</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="10"/>
+        <v>378</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="11"/>
+        <v>350</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="12"/>
+        <v>622</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31">
+        <v>800</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>80</v>
+      </c>
+      <c r="H31">
+        <v>1.08</v>
+      </c>
+      <c r="I31">
+        <v>1.25</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="9"/>
+        <v>400</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="10"/>
+        <v>432</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="11"/>
+        <v>400</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="12"/>
+        <v>568</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32">
+        <v>900</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="15"/>
+        <v>11.25</v>
+      </c>
+      <c r="F32">
+        <v>80</v>
+      </c>
+      <c r="H32">
+        <v>1.08</v>
+      </c>
+      <c r="I32">
+        <v>1.25</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="9"/>
+        <v>450</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="10"/>
+        <v>486.00000000000006</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="11"/>
+        <v>450</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="12"/>
+        <v>514</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="13"/>
+        <v>38.800000000000011</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>1000</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="15"/>
+        <v>12.5</v>
+      </c>
+      <c r="F33">
+        <v>80</v>
+      </c>
+      <c r="H33">
+        <v>1.08</v>
+      </c>
+      <c r="I33">
+        <v>1.25</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="9"/>
+        <v>500</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="10"/>
+        <v>540</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="11"/>
+        <v>500</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="12"/>
+        <v>460</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="13"/>
+        <v>132</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="14"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>1000</v>
+      </c>
+      <c r="D34">
+        <v>1200</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <v>80</v>
+      </c>
+      <c r="H34">
+        <v>1.08</v>
+      </c>
+      <c r="I34">
+        <v>1.25</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="9"/>
+        <v>600</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="10"/>
+        <v>648</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="11"/>
+        <v>600</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="12"/>
+        <v>352</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="13"/>
+        <v>318.39999999999998</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="14"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35">
+        <v>514</v>
+      </c>
+      <c r="D35">
+        <v>450</v>
+      </c>
+      <c r="H35">
+        <v>1.08</v>
+      </c>
+      <c r="I35">
+        <v>1.25</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="9"/>
+        <v>225</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="10"/>
+        <v>243.00000000000003</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="11"/>
+        <v>225</v>
+      </c>
+      <c r="M35">
+        <f>C35-K35</f>
+        <v>271</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="13"/>
+        <v>8.1999999999999886</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="14"/>
+        <v>38.800000000000011</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>271</v>
+      </c>
+      <c r="D36">
+        <v>225</v>
+      </c>
+      <c r="H36">
+        <v>1.08</v>
+      </c>
+      <c r="I36">
+        <v>1.25</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="9"/>
+        <v>112.5</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="10"/>
+        <v>121.50000000000001</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="11"/>
+        <v>112.5</v>
+      </c>
+      <c r="M36">
+        <f>C36-K36</f>
+        <v>149.5</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="14"/>
+        <v>8.1999999999999886</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C20:E20"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>